<commit_message>
testing if comments hidden
</commit_message>
<xml_diff>
--- a/output/out_2023-10-31T12:24:03.598/decompositions/decompositions_combined.xlsx
+++ b/output/out_2023-10-31T12:24:03.598/decompositions/decompositions_combined.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10513"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felipenoris/tmp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chaseabram/UChiGit/seq-auction-firm-dyn/output/out_2023-10-31T12:24:03.598/decompositions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C353BCB8-5EC8-0143-BDD3-A1B661DAACD7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C7EAF1-5361-3B45-B8BB-3FAEE672F518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
+    <workbookView xWindow="380" yWindow="740" windowWidth="28040" windowHeight="17040" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
   </bookViews>
   <sheets>
-    <sheet name="params" sheetId="1" r:id="rId1"/>
+    <sheet name="decomps" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="60">
   <si>
     <t>anzsic</t>
   </si>
@@ -558,11 +558,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
   <dimension ref="A1:J270"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -594,7 +596,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -602,31 +604,31 @@
         <v>11</v>
       </c>
       <c r="C6">
-        <v>0.028290050591672538</v>
+        <v>2.8290050591672538E-2</v>
       </c>
       <c r="D6">
-        <v>0.011986028934225257</v>
+        <v>1.1986028934225257E-2</v>
       </c>
       <c r="E6">
-        <v>0.012730830144434156</v>
+        <v>1.2730830144434156E-2</v>
       </c>
       <c r="F6">
-        <v>0.021692226780980487</v>
+        <v>2.1692226780980487E-2</v>
       </c>
       <c r="G6">
         <v>0.9543179452372299</v>
       </c>
       <c r="H6">
-        <v>0.04568205476277024</v>
+        <v>4.5682054762770243E-2</v>
       </c>
       <c r="I6">
         <v>0.4046746225756101</v>
       </c>
       <c r="J6">
-        <v>0.59532537742439</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>0.59532537742438996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -634,31 +636,31 @@
         <v>11</v>
       </c>
       <c r="C8">
-        <v>0.025603393905940432</v>
+        <v>2.5603393905940432E-2</v>
       </c>
       <c r="D8">
-        <v>0.013496948199188468</v>
+        <v>1.3496948199188468E-2</v>
       </c>
       <c r="E8">
-        <v>0.015345092564714483</v>
+        <v>1.5345092564714483E-2</v>
       </c>
       <c r="F8">
-        <v>0.019594075412784046</v>
+        <v>1.9594075412784046E-2</v>
       </c>
       <c r="G8">
-        <v>0.8473421175551735</v>
+        <v>0.84734211755517352</v>
       </c>
       <c r="H8">
         <v>0.15265788244482645</v>
       </c>
       <c r="I8">
-        <v>0.4963734723400189</v>
+        <v>0.49637347234001888</v>
       </c>
       <c r="J8">
-        <v>0.5036265276599811</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+        <v>0.50362652765998106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -666,31 +668,31 @@
         <v>11</v>
       </c>
       <c r="C14">
-        <v>0.03506260829158053</v>
+        <v>3.5062608291580533E-2</v>
       </c>
       <c r="D14">
-        <v>0.019747119704225626</v>
+        <v>1.9747119704225626E-2</v>
       </c>
       <c r="E14">
-        <v>0.025608000400050252</v>
+        <v>2.5608000400050252E-2</v>
       </c>
       <c r="F14">
-        <v>0.027496368736896957</v>
+        <v>2.7496368736896957E-2</v>
       </c>
       <c r="G14">
-        <v>0.6173232957998083</v>
+        <v>0.61732329579980827</v>
       </c>
       <c r="H14">
         <v>0.38267670420019173</v>
       </c>
       <c r="I14">
-        <v>0.4940253464019798</v>
+        <v>0.49402534640197981</v>
       </c>
       <c r="J14">
-        <v>0.5059746535980202</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
+        <v>0.50597465359802019</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>46</v>
       </c>
@@ -698,31 +700,31 @@
         <v>11</v>
       </c>
       <c r="C26">
-        <v>0.022737387790981913</v>
+        <v>2.2737387790981913E-2</v>
       </c>
       <c r="D26">
-        <v>0.014079381232265684</v>
+        <v>1.4079381232265684E-2</v>
       </c>
       <c r="E26">
-        <v>0.01672603140184349</v>
+        <v>1.6726031401843491E-2</v>
       </c>
       <c r="F26">
-        <v>0.019964264607983607</v>
+        <v>1.9964264607983607E-2</v>
       </c>
       <c r="G26">
-        <v>0.6943118312940801</v>
+        <v>0.69431183129408014</v>
       </c>
       <c r="H26">
         <v>0.30568816870591986</v>
       </c>
       <c r="I26">
-        <v>0.320295805297876</v>
+        <v>0.32029580529787599</v>
       </c>
       <c r="J26">
-        <v>0.6797041947021241</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
+        <v>0.67970419470212406</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>51</v>
       </c>
@@ -730,31 +732,31 @@
         <v>11</v>
       </c>
       <c r="C30">
-        <v>0.026463389021870856</v>
+        <v>2.6463389021870856E-2</v>
       </c>
       <c r="D30">
-        <v>0.013445189386869292</v>
+        <v>1.3445189386869292E-2</v>
       </c>
       <c r="E30">
-        <v>0.017227226015234152</v>
+        <v>1.7227226015234152E-2</v>
       </c>
       <c r="F30">
-        <v>0.022757343165058577</v>
+        <v>2.2757343165058577E-2</v>
       </c>
       <c r="G30">
-        <v>0.7094808241996662</v>
+        <v>0.70948082419966618</v>
       </c>
       <c r="H30">
-        <v>0.2905191758003338</v>
+        <v>0.29051917580033382</v>
       </c>
       <c r="I30">
         <v>0.28468190385158687</v>
       </c>
       <c r="J30">
-        <v>0.7153180961484131</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10">
+        <v>0.71531809614841313</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>52</v>
       </c>
@@ -762,31 +764,31 @@
         <v>11</v>
       </c>
       <c r="C34">
-        <v>0.020381123546134545</v>
+        <v>2.0381123546134545E-2</v>
       </c>
       <c r="D34">
-        <v>0.02121183153653404</v>
+        <v>2.121183153653404E-2</v>
       </c>
       <c r="E34">
-        <v>0.021163671386061785</v>
+        <v>2.1163671386061785E-2</v>
       </c>
       <c r="F34">
-        <v>0.01865155752962987</v>
+        <v>1.865155752962987E-2</v>
       </c>
       <c r="G34">
-        <v>0.9420251748763196</v>
+        <v>0.94202517487631965</v>
       </c>
       <c r="H34">
-        <v>0.05797482512368036</v>
+        <v>5.7974825123680358E-2</v>
       </c>
       <c r="I34">
-        <v>-2.082038497875662</v>
+        <v>-2.0820384978756619</v>
       </c>
       <c r="J34">
-        <v>3.082038497875662</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10">
+        <v>3.0820384978756619</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>53</v>
       </c>
@@ -794,31 +796,31 @@
         <v>11</v>
       </c>
       <c r="C48">
-        <v>0.044532511707619044</v>
+        <v>4.4532511707619044E-2</v>
       </c>
       <c r="D48">
-        <v>0.02441746214321755</v>
+        <v>2.441746214321755E-2</v>
       </c>
       <c r="E48">
-        <v>0.026995988528153714</v>
+        <v>2.6995988528153714E-2</v>
       </c>
       <c r="F48">
-        <v>0.03889753980678378</v>
+        <v>3.889753980678378E-2</v>
       </c>
       <c r="G48">
-        <v>0.87181108469653</v>
+        <v>0.87181108469653001</v>
       </c>
       <c r="H48">
         <v>0.12818891530346999</v>
       </c>
       <c r="I48">
-        <v>0.2801371124040244</v>
+        <v>0.28013711240402439</v>
       </c>
       <c r="J48">
-        <v>0.7198628875959756</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10">
+        <v>0.71986288759597561</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>55</v>
       </c>
@@ -826,16 +828,16 @@
         <v>11</v>
       </c>
       <c r="C64">
-        <v>0.02840050139716296</v>
+        <v>2.840050139716296E-2</v>
       </c>
       <c r="D64">
-        <v>0.01895662172066619</v>
+        <v>1.895662172066619E-2</v>
       </c>
       <c r="E64">
-        <v>0.021022103367057926</v>
+        <v>2.1022103367057926E-2</v>
       </c>
       <c r="F64">
-        <v>0.02470107168744845</v>
+        <v>2.470107168744845E-2</v>
       </c>
       <c r="G64">
         <v>0.7812888646249746</v>
@@ -847,10 +849,10 @@
         <v>0.39172774711661956</v>
       </c>
       <c r="J64">
-        <v>0.6082722528833804</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10">
+        <v>0.60827225288338038</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>57</v>
       </c>
@@ -858,31 +860,31 @@
         <v>11</v>
       </c>
       <c r="C82">
-        <v>0.02481129423031391</v>
+        <v>2.4811294230313911E-2</v>
       </c>
       <c r="D82">
-        <v>0.014460123410305557</v>
+        <v>1.4460123410305557E-2</v>
       </c>
       <c r="E82">
-        <v>0.01683508186169781</v>
+        <v>1.6835081861697809E-2</v>
       </c>
       <c r="F82">
-        <v>0.02162447039032776</v>
+        <v>2.162447039032776E-2</v>
       </c>
       <c r="G82">
-        <v>0.7705613700431296</v>
+        <v>0.77056137004312963</v>
       </c>
       <c r="H82">
-        <v>0.2294386299568704</v>
+        <v>0.22943862995687039</v>
       </c>
       <c r="I82">
-        <v>0.3078708578382421</v>
+        <v>0.30787085783824208</v>
       </c>
       <c r="J82">
-        <v>0.6921291421617579</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10">
+        <v>0.69212914216175792</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>58</v>
       </c>
@@ -890,31 +892,31 @@
         <v>11</v>
       </c>
       <c r="C92">
-        <v>0.018185670156493798</v>
+        <v>1.8185670156493798E-2</v>
       </c>
       <c r="D92">
-        <v>0.014949479801722987</v>
+        <v>1.4949479801722987E-2</v>
       </c>
       <c r="E92">
-        <v>0.015324053569582987</v>
+        <v>1.5324053569582987E-2</v>
       </c>
       <c r="F92">
-        <v>0.016496642083774292</v>
+        <v>1.6496642083774292E-2</v>
       </c>
       <c r="G92">
-        <v>0.8842547171838017</v>
+        <v>0.88425471718380166</v>
       </c>
       <c r="H92">
         <v>0.11574528281619835</v>
       </c>
       <c r="I92">
-        <v>0.5219186412287308</v>
+        <v>0.52191864122873077</v>
       </c>
       <c r="J92">
-        <v>0.4780813587712692</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10">
+        <v>0.47808135877126923</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>59</v>
       </c>
@@ -922,16 +924,16 @@
         <v>11</v>
       </c>
       <c r="C96">
-        <v>0.01783532781371527</v>
+        <v>1.783532781371527E-2</v>
       </c>
       <c r="D96">
-        <v>0.028086440790785958</v>
+        <v>2.8086440790785958E-2</v>
       </c>
       <c r="E96">
-        <v>0.03014792496159481</v>
+        <v>3.014792496159481E-2</v>
       </c>
       <c r="F96">
-        <v>0.01755203692210964</v>
+        <v>1.7552036922109639E-2</v>
       </c>
       <c r="G96">
         <v>1.201098570996135</v>
@@ -940,13 +942,13 @@
         <v>-0.20109857099613515</v>
       </c>
       <c r="I96">
-        <v>-0.027635135056972474</v>
+        <v>-2.7635135056972474E-2</v>
       </c>
       <c r="J96">
         <v>1.0276351350569726</v>
       </c>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>10</v>
       </c>
@@ -954,31 +956,31 @@
         <v>11</v>
       </c>
       <c r="C102">
-        <v>0.026142232117825865</v>
+        <v>2.6142232117825865E-2</v>
       </c>
       <c r="D102">
-        <v>0.019307511827295065</v>
+        <v>1.9307511827295065E-2</v>
       </c>
       <c r="E102">
-        <v>0.020451888374320364</v>
+        <v>2.0451888374320364E-2</v>
       </c>
       <c r="F102">
-        <v>0.025969357540292504</v>
+        <v>2.5969357540292504E-2</v>
       </c>
       <c r="G102">
-        <v>0.8325642457364668</v>
+        <v>0.83256424573646681</v>
       </c>
       <c r="H102">
-        <v>0.1674357542635332</v>
+        <v>0.16743575426353319</v>
       </c>
       <c r="I102">
-        <v>0.025293584841046293</v>
+        <v>2.5293584841046293E-2</v>
       </c>
       <c r="J102">
-        <v>0.9747064151589537</v>
-      </c>
-    </row>
-    <row r="126" spans="1:10">
+        <v>0.97470641515895373</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>12</v>
       </c>
@@ -986,31 +988,31 @@
         <v>11</v>
       </c>
       <c r="C126">
-        <v>0.010702197458744183</v>
+        <v>1.0702197458744183E-2</v>
       </c>
       <c r="D126">
-        <v>0.014489970622175729</v>
+        <v>1.4489970622175729E-2</v>
       </c>
       <c r="E126">
-        <v>0.013831830908856656</v>
+        <v>1.3831830908856656E-2</v>
       </c>
       <c r="F126">
-        <v>0.01039604879854869</v>
+        <v>1.039604879854869E-2</v>
       </c>
       <c r="G126">
-        <v>0.8262462705863757</v>
+        <v>0.82624627058637568</v>
       </c>
       <c r="H126">
         <v>0.1737537294136243</v>
       </c>
       <c r="I126">
-        <v>-0.08082550009888567</v>
+        <v>-8.0825500098885672E-2</v>
       </c>
       <c r="J126">
         <v>1.0808255000988858</v>
       </c>
     </row>
-    <row r="130" spans="1:10">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>13</v>
       </c>
@@ -1018,31 +1020,31 @@
         <v>11</v>
       </c>
       <c r="C130">
-        <v>0.011938588137422785</v>
+        <v>1.1938588137422785E-2</v>
       </c>
       <c r="D130">
-        <v>0.018767283867544875</v>
+        <v>1.8767283867544875E-2</v>
       </c>
       <c r="E130">
-        <v>0.015768365481064923</v>
+        <v>1.5768365481064923E-2</v>
       </c>
       <c r="F130">
-        <v>0.012194322713607202</v>
+        <v>1.2194322713607202E-2</v>
       </c>
       <c r="G130">
-        <v>0.5608358455259019</v>
+        <v>0.56083584552590193</v>
       </c>
       <c r="H130">
-        <v>0.4391641544740981</v>
+        <v>0.43916415447409812</v>
       </c>
       <c r="I130">
-        <v>0.037449988444549484</v>
+        <v>3.7449988444549484E-2</v>
       </c>
       <c r="J130">
         <v>0.9625500115554505</v>
       </c>
     </row>
-    <row r="132" spans="1:10">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>14</v>
       </c>
@@ -1050,31 +1052,31 @@
         <v>11</v>
       </c>
       <c r="C132">
-        <v>0.030417052890020575</v>
+        <v>3.0417052890020575E-2</v>
       </c>
       <c r="D132">
-        <v>0.010217165010941432</v>
+        <v>1.0217165010941432E-2</v>
       </c>
       <c r="E132">
-        <v>0.010845365454236167</v>
+        <v>1.0845365454236167E-2</v>
       </c>
       <c r="F132">
-        <v>0.02345537199675124</v>
+        <v>2.345537199675124E-2</v>
       </c>
       <c r="G132">
         <v>0.9689007955363278</v>
       </c>
       <c r="H132">
-        <v>0.031099204463672144</v>
+        <v>3.1099204463672144E-2</v>
       </c>
       <c r="I132">
         <v>0.34463958091962926</v>
       </c>
       <c r="J132">
-        <v>0.6553604190803707</v>
-      </c>
-    </row>
-    <row r="140" spans="1:10">
+        <v>0.65536041908037068</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>16</v>
       </c>
@@ -1082,31 +1084,31 @@
         <v>11</v>
       </c>
       <c r="C140">
-        <v>0.03022970446471194</v>
+        <v>3.0229704464711939E-2</v>
       </c>
       <c r="D140">
-        <v>0.015094888927481846</v>
+        <v>1.5094888927481846E-2</v>
       </c>
       <c r="E140">
-        <v>0.019465232356876732</v>
+        <v>1.9465232356876732E-2</v>
       </c>
       <c r="F140">
-        <v>0.022319456097946458</v>
+        <v>2.2319456097946458E-2</v>
       </c>
       <c r="G140">
-        <v>0.7112390687125132</v>
+        <v>0.71123906871251319</v>
       </c>
       <c r="H140">
-        <v>0.2887609312874868</v>
+        <v>0.28876093128748681</v>
       </c>
       <c r="I140">
-        <v>0.5226524464277137</v>
+        <v>0.52265244642771369</v>
       </c>
       <c r="J140">
         <v>0.47734755357228625</v>
       </c>
     </row>
-    <row r="148" spans="1:10">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>17</v>
       </c>
@@ -1114,31 +1116,31 @@
         <v>11</v>
       </c>
       <c r="C148">
-        <v>0.027103354108057316</v>
+        <v>2.7103354108057316E-2</v>
       </c>
       <c r="D148">
-        <v>0.02338020073180386</v>
+        <v>2.3380200731803861E-2</v>
       </c>
       <c r="E148">
-        <v>0.025592665189301686</v>
+        <v>2.5592665189301686E-2</v>
       </c>
       <c r="F148">
-        <v>0.025808176179307016</v>
+        <v>2.5808176179307016E-2</v>
       </c>
       <c r="G148">
         <v>0.40575522039755724</v>
       </c>
       <c r="H148">
-        <v>0.5942447796024427</v>
+        <v>0.59424477960244271</v>
       </c>
       <c r="I148">
-        <v>0.3478712257762573</v>
+        <v>0.34787122577625729</v>
       </c>
       <c r="J148">
-        <v>0.6521287742237427</v>
-      </c>
-    </row>
-    <row r="150" spans="1:10">
+        <v>0.65212877422374271</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>18</v>
       </c>
@@ -1146,16 +1148,16 @@
         <v>11</v>
       </c>
       <c r="C150">
-        <v>0.02096825300953771</v>
+        <v>2.096825300953771E-2</v>
       </c>
       <c r="D150">
-        <v>0.01940359014718922</v>
+        <v>1.9403590147189221E-2</v>
       </c>
       <c r="E150">
-        <v>0.02044217881798621</v>
+        <v>2.0442178817986208E-2</v>
       </c>
       <c r="F150">
-        <v>0.020807888816857096</v>
+        <v>2.0807888816857096E-2</v>
       </c>
       <c r="G150">
         <v>0.3362220732726332</v>
@@ -1167,10 +1169,10 @@
         <v>0.10249121171056279</v>
       </c>
       <c r="J150">
-        <v>0.8975087882894373</v>
-      </c>
-    </row>
-    <row r="152" spans="1:10">
+        <v>0.89750878828943725</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>19</v>
       </c>
@@ -1178,31 +1180,31 @@
         <v>11</v>
       </c>
       <c r="C152">
-        <v>0.013120605153750742</v>
+        <v>1.3120605153750742E-2</v>
       </c>
       <c r="D152">
-        <v>0.024055289763075294</v>
+        <v>2.4055289763075294E-2</v>
       </c>
       <c r="E152">
-        <v>0.023959084669321454</v>
+        <v>2.3959084669321454E-2</v>
       </c>
       <c r="F152">
-        <v>0.013575581948185044</v>
+        <v>1.3575581948185044E-2</v>
       </c>
       <c r="G152">
         <v>0.9912018410049247</v>
       </c>
       <c r="H152">
-        <v>0.008798158995075278</v>
+        <v>8.7981589950752778E-3</v>
       </c>
       <c r="I152">
-        <v>0.04160858869640564</v>
+        <v>4.1608588696405643E-2</v>
       </c>
       <c r="J152">
         <v>0.9583914113035944</v>
       </c>
     </row>
-    <row r="154" spans="1:10">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>20</v>
       </c>
@@ -1210,19 +1212,19 @@
         <v>11</v>
       </c>
       <c r="C154">
-        <v>0.023084527837897786</v>
+        <v>2.3084527837897786E-2</v>
       </c>
       <c r="D154">
-        <v>0.0279658054877986</v>
+        <v>2.79658054877986E-2</v>
       </c>
       <c r="E154">
-        <v>0.026899766591455498</v>
+        <v>2.6899766591455498E-2</v>
       </c>
       <c r="F154">
-        <v>0.025470517223146336</v>
+        <v>2.5470517223146336E-2</v>
       </c>
       <c r="G154">
-        <v>0.7816065848324026</v>
+        <v>0.78160658483240264</v>
       </c>
       <c r="H154">
         <v>0.21839341516759733</v>
@@ -1231,10 +1233,10 @@
         <v>0.48880427551525013</v>
       </c>
       <c r="J154">
-        <v>0.5111957244847499</v>
-      </c>
-    </row>
-    <row r="158" spans="1:10">
+        <v>0.51119572448474992</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>21</v>
       </c>
@@ -1242,22 +1244,22 @@
         <v>11</v>
       </c>
       <c r="C158">
-        <v>0.015404778851365947</v>
+        <v>1.5404778851365947E-2</v>
       </c>
       <c r="D158">
-        <v>0.01247179229992499</v>
+        <v>1.247179229992499E-2</v>
       </c>
       <c r="E158">
-        <v>0.014780123105626973</v>
+        <v>1.4780123105626973E-2</v>
       </c>
       <c r="F158">
-        <v>0.014068313894899237</v>
+        <v>1.4068313894899237E-2</v>
       </c>
       <c r="G158">
         <v>0.21297600066801695</v>
       </c>
       <c r="H158">
-        <v>0.7870239993319831</v>
+        <v>0.78702399933198308</v>
       </c>
       <c r="I158">
         <v>0.4556669227856206</v>
@@ -1266,7 +1268,7 @@
         <v>0.5443330772143794</v>
       </c>
     </row>
-    <row r="164" spans="1:10">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>22</v>
       </c>
@@ -1274,31 +1276,31 @@
         <v>11</v>
       </c>
       <c r="C164">
-        <v>0.02086896817748563</v>
+        <v>2.0868968177485629E-2</v>
       </c>
       <c r="D164">
-        <v>0.014639309929276428</v>
+        <v>1.4639309929276428E-2</v>
       </c>
       <c r="E164">
-        <v>0.017041063158184915</v>
+        <v>1.7041063158184915E-2</v>
       </c>
       <c r="F164">
-        <v>0.017543578580932088</v>
+        <v>1.7543578580932088E-2</v>
       </c>
       <c r="G164">
-        <v>0.614464689198817</v>
+        <v>0.61446468919881703</v>
       </c>
       <c r="H164">
-        <v>0.385535310801183</v>
+        <v>0.38553531080118297</v>
       </c>
       <c r="I164">
-        <v>0.5337996827529775</v>
+        <v>0.53379968275297751</v>
       </c>
       <c r="J164">
-        <v>0.4662003172470225</v>
-      </c>
-    </row>
-    <row r="166" spans="1:10">
+        <v>0.46620031724702249</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>23</v>
       </c>
@@ -1306,19 +1308,19 @@
         <v>11</v>
       </c>
       <c r="C166">
-        <v>0.00845526522295936</v>
+        <v>8.4552652229593593E-3</v>
       </c>
       <c r="D166">
-        <v>0.0168846520962143</v>
+        <v>1.68846520962143E-2</v>
       </c>
       <c r="E166">
-        <v>0.012896585644155476</v>
+        <v>1.2896585644155476E-2</v>
       </c>
       <c r="F166">
-        <v>0.010838413522643501</v>
+        <v>1.0838413522643501E-2</v>
       </c>
       <c r="G166">
-        <v>0.5268853462269831</v>
+        <v>0.52688534622698313</v>
       </c>
       <c r="H166">
         <v>0.47311465377301687</v>
@@ -1327,10 +1329,10 @@
         <v>0.28271905602594655</v>
       </c>
       <c r="J166">
-        <v>0.7172809439740535</v>
-      </c>
-    </row>
-    <row r="168" spans="1:10">
+        <v>0.71728094397405351</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>24</v>
       </c>
@@ -1338,16 +1340,16 @@
         <v>11</v>
       </c>
       <c r="C168">
-        <v>0.01049743416877182</v>
+        <v>1.0497434168771819E-2</v>
       </c>
       <c r="D168">
-        <v>0.010464352164986113</v>
+        <v>1.0464352164986113E-2</v>
       </c>
       <c r="E168">
-        <v>0.011217222849796848</v>
+        <v>1.1217222849796848E-2</v>
       </c>
       <c r="F168">
-        <v>0.008706975708737389</v>
+        <v>8.7069757087373887E-3</v>
       </c>
       <c r="G168">
         <v>-21.757711101406297</v>
@@ -1356,13 +1358,13 @@
         <v>22.757711101406297</v>
       </c>
       <c r="I168">
-        <v>54.12182622408223</v>
+        <v>54.121826224082227</v>
       </c>
       <c r="J168">
-        <v>-53.12182622408223</v>
-      </c>
-    </row>
-    <row r="170" spans="1:10">
+        <v>-53.121826224082227</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>25</v>
       </c>
@@ -1370,19 +1372,19 @@
         <v>11</v>
       </c>
       <c r="C170">
-        <v>0.018194638545837968</v>
+        <v>1.8194638545837968E-2</v>
       </c>
       <c r="D170">
-        <v>0.02134449721969241</v>
+        <v>2.1344497219692411E-2</v>
       </c>
       <c r="E170">
-        <v>0.020617971647203182</v>
+        <v>2.0617971647203182E-2</v>
       </c>
       <c r="F170">
-        <v>0.018844351518637496</v>
+        <v>1.8844351518637496E-2</v>
       </c>
       <c r="G170">
-        <v>0.7693466127481243</v>
+        <v>0.76934661274812433</v>
       </c>
       <c r="H170">
         <v>0.23065338725187565</v>
@@ -1391,10 +1393,10 @@
         <v>0.20626734087865692</v>
       </c>
       <c r="J170">
-        <v>0.793732659121343</v>
-      </c>
-    </row>
-    <row r="192" spans="1:10">
+        <v>0.79373265912134305</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>26</v>
       </c>
@@ -1402,16 +1404,16 @@
         <v>11</v>
       </c>
       <c r="C192">
-        <v>0.02033943403363542</v>
+        <v>2.0339434033635421E-2</v>
       </c>
       <c r="D192">
-        <v>0.022422020149504524</v>
+        <v>2.2422020149504524E-2</v>
       </c>
       <c r="E192">
-        <v>0.022064570655747188</v>
+        <v>2.2064570655747188E-2</v>
       </c>
       <c r="F192">
-        <v>0.019744388158429833</v>
+        <v>1.9744388158429833E-2</v>
       </c>
       <c r="G192">
         <v>0.8283626828040358</v>
@@ -1420,13 +1422,13 @@
         <v>0.1716373171959642</v>
       </c>
       <c r="I192">
-        <v>-0.2857244992998829</v>
+        <v>-0.28572449929988292</v>
       </c>
       <c r="J192">
         <v>1.2857244992998829</v>
       </c>
     </row>
-    <row r="196" spans="1:10">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>27</v>
       </c>
@@ -1434,31 +1436,31 @@
         <v>11</v>
       </c>
       <c r="C196">
-        <v>0.02364641268653471</v>
+        <v>2.364641268653471E-2</v>
       </c>
       <c r="D196">
-        <v>0.018853736966658267</v>
+        <v>1.8853736966658267E-2</v>
       </c>
       <c r="E196">
-        <v>0.020728279143259636</v>
+        <v>2.0728279143259636E-2</v>
       </c>
       <c r="F196">
-        <v>0.022163031456866242</v>
+        <v>2.2163031456866242E-2</v>
       </c>
       <c r="G196">
-        <v>0.6088735632942646</v>
+        <v>0.60887356329426456</v>
       </c>
       <c r="H196">
-        <v>0.3911264367057355</v>
+        <v>0.39112643670573549</v>
       </c>
       <c r="I196">
-        <v>0.3095100349720113</v>
+        <v>0.30951003497201129</v>
       </c>
       <c r="J196">
-        <v>0.6904899650279888</v>
-      </c>
-    </row>
-    <row r="200" spans="1:10">
+        <v>0.69048996502798876</v>
+      </c>
+    </row>
+    <row r="200" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>28</v>
       </c>
@@ -1466,22 +1468,22 @@
         <v>11</v>
       </c>
       <c r="C200">
-        <v>0.016764869305684882</v>
+        <v>1.6764869305684882E-2</v>
       </c>
       <c r="D200">
-        <v>0.019157974473851796</v>
+        <v>1.9157974473851796E-2</v>
       </c>
       <c r="E200">
-        <v>0.019240510940989046</v>
+        <v>1.9240510940989046E-2</v>
       </c>
       <c r="F200">
-        <v>0.0174576416238517</v>
+        <v>1.7457641623851699E-2</v>
       </c>
       <c r="G200">
-        <v>1.03448927704271</v>
+        <v>1.0344892770427101</v>
       </c>
       <c r="H200">
-        <v>-0.03448927704271014</v>
+        <v>-3.448927704271014E-2</v>
       </c>
       <c r="I200">
         <v>0.2894867836909446</v>
@@ -1490,7 +1492,7 @@
         <v>0.7105132163090554</v>
       </c>
     </row>
-    <row r="202" spans="1:10">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>29</v>
       </c>
@@ -1498,19 +1500,19 @@
         <v>11</v>
       </c>
       <c r="C202">
-        <v>0.020418614962466747</v>
+        <v>2.0418614962466747E-2</v>
       </c>
       <c r="D202">
-        <v>0.007861019739531712</v>
+        <v>7.8610197395317122E-3</v>
       </c>
       <c r="E202">
-        <v>0.010431023767657808</v>
+        <v>1.0431023767657808E-2</v>
       </c>
       <c r="F202">
-        <v>0.01664203489296585</v>
+        <v>1.6642034892965851E-2</v>
       </c>
       <c r="G202">
-        <v>0.7953426605571525</v>
+        <v>0.79534266055715253</v>
       </c>
       <c r="H202">
         <v>0.20465733944284753</v>
@@ -1522,7 +1524,7 @@
         <v>0.6992592926865967</v>
       </c>
     </row>
-    <row r="212" spans="1:10">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>30</v>
       </c>
@@ -1530,31 +1532,31 @@
         <v>11</v>
       </c>
       <c r="C212">
-        <v>0.02015560194112895</v>
+        <v>2.0155601941128951E-2</v>
       </c>
       <c r="D212">
-        <v>0.015227093332475364</v>
+        <v>1.5227093332475364E-2</v>
       </c>
       <c r="E212">
-        <v>0.01861612362666609</v>
+        <v>1.8616123626666089E-2</v>
       </c>
       <c r="F212">
-        <v>0.018004621149553146</v>
+        <v>1.8004621149553146E-2</v>
       </c>
       <c r="G212">
         <v>0.31236190026325844</v>
       </c>
       <c r="H212">
-        <v>0.6876380997367416</v>
+        <v>0.68763809973674161</v>
       </c>
       <c r="I212">
         <v>0.4364364480969079</v>
       </c>
       <c r="J212">
-        <v>0.5635635519030922</v>
-      </c>
-    </row>
-    <row r="214" spans="1:10">
+        <v>0.56356355190309215</v>
+      </c>
+    </row>
+    <row r="214" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>31</v>
       </c>
@@ -1562,16 +1564,16 @@
         <v>11</v>
       </c>
       <c r="C214">
-        <v>0.013718047524076425</v>
+        <v>1.3718047524076425E-2</v>
       </c>
       <c r="D214">
-        <v>0.016182803194331706</v>
+        <v>1.6182803194331706E-2</v>
       </c>
       <c r="E214">
-        <v>0.016754779107695045</v>
+        <v>1.6754779107695045E-2</v>
       </c>
       <c r="F214">
-        <v>0.012959755050947612</v>
+        <v>1.2959755050947612E-2</v>
       </c>
       <c r="G214">
         <v>1.232061911963914</v>
@@ -1586,7 +1588,7 @@
         <v>1.3076542159046032</v>
       </c>
     </row>
-    <row r="216" spans="1:10">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>32</v>
       </c>
@@ -1594,31 +1596,31 @@
         <v>11</v>
       </c>
       <c r="C216">
-        <v>0.03060029274931026</v>
+        <v>3.0600292749310261E-2</v>
       </c>
       <c r="D216">
-        <v>0.012911725639797929</v>
+        <v>1.2911725639797929E-2</v>
       </c>
       <c r="E216">
-        <v>0.015996636307566623</v>
+        <v>1.5996636307566623E-2</v>
       </c>
       <c r="F216">
-        <v>0.026721024561157724</v>
+        <v>2.6721024561157724E-2</v>
       </c>
       <c r="G216">
-        <v>0.8255986113137603</v>
+        <v>0.82559861131376033</v>
       </c>
       <c r="H216">
-        <v>0.1744013886862396</v>
+        <v>0.17440138868623961</v>
       </c>
       <c r="I216">
         <v>0.21930935186188108</v>
       </c>
       <c r="J216">
-        <v>0.780690648138119</v>
-      </c>
-    </row>
-    <row r="218" spans="1:10">
+        <v>0.78069064813811895</v>
+      </c>
+    </row>
+    <row r="218" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>33</v>
       </c>
@@ -1626,22 +1628,22 @@
         <v>11</v>
       </c>
       <c r="C218">
-        <v>0.021432779802765707</v>
+        <v>2.1432779802765707E-2</v>
       </c>
       <c r="D218">
-        <v>0.017122710826888238</v>
+        <v>1.7122710826888238E-2</v>
       </c>
       <c r="E218">
-        <v>0.018936477711922754</v>
+        <v>1.8936477711922754E-2</v>
       </c>
       <c r="F218">
-        <v>0.022180719020458917</v>
+        <v>2.2180719020458917E-2</v>
       </c>
       <c r="G218">
-        <v>0.5791791511491394</v>
+        <v>0.57917915114913943</v>
       </c>
       <c r="H218">
-        <v>0.4208208488508605</v>
+        <v>0.42082084885086052</v>
       </c>
       <c r="I218">
         <v>-0.17353300419999435</v>
@@ -1650,7 +1652,7 @@
         <v>1.1735330041999943</v>
       </c>
     </row>
-    <row r="222" spans="1:10">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>34</v>
       </c>
@@ -1658,22 +1660,22 @@
         <v>11</v>
       </c>
       <c r="C222">
-        <v>0.01898305879604807</v>
+        <v>1.8983058796048068E-2</v>
       </c>
       <c r="D222">
-        <v>0.01544238909848441</v>
+        <v>1.5442389098484411E-2</v>
       </c>
       <c r="E222">
-        <v>0.017393464804400287</v>
+        <v>1.7393464804400287E-2</v>
       </c>
       <c r="F222">
-        <v>0.0198171744442564</v>
+        <v>1.9817174444256399E-2</v>
       </c>
       <c r="G222">
-        <v>0.4489529177888535</v>
+        <v>0.44895291778885349</v>
       </c>
       <c r="H222">
-        <v>0.5510470822111465</v>
+        <v>0.55104708221114651</v>
       </c>
       <c r="I222">
         <v>-0.23558132202568552</v>
@@ -1682,7 +1684,7 @@
         <v>1.2355813220256855</v>
       </c>
     </row>
-    <row r="226" spans="1:10">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>35</v>
       </c>
@@ -1690,31 +1692,31 @@
         <v>11</v>
       </c>
       <c r="C226">
-        <v>0.031366882544836765</v>
+        <v>3.1366882544836765E-2</v>
       </c>
       <c r="D226">
-        <v>0.03710441015620168</v>
+        <v>3.7104410156201681E-2</v>
       </c>
       <c r="E226">
-        <v>0.03861656891720806</v>
+        <v>3.8616568917208063E-2</v>
       </c>
       <c r="F226">
-        <v>0.030497259054287906</v>
+        <v>3.0497259054287906E-2</v>
       </c>
       <c r="G226">
         <v>1.2635558141822434</v>
       </c>
       <c r="H226">
-        <v>-0.2635558141822434</v>
+        <v>-0.26355581418224339</v>
       </c>
       <c r="I226">
         <v>-0.1515676349559181</v>
       </c>
       <c r="J226">
-        <v>1.151567634955918</v>
-      </c>
-    </row>
-    <row r="228" spans="1:10">
+        <v>1.1515676349559181</v>
+      </c>
+    </row>
+    <row r="228" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>36</v>
       </c>
@@ -1722,22 +1724,22 @@
         <v>11</v>
       </c>
       <c r="C228">
-        <v>0.013669569265524664</v>
+        <v>1.3669569265524664E-2</v>
       </c>
       <c r="D228">
-        <v>0.019169428495765934</v>
+        <v>1.9169428495765934E-2</v>
       </c>
       <c r="E228">
-        <v>0.017622445935001115</v>
+        <v>1.7622445935001115E-2</v>
       </c>
       <c r="F228">
-        <v>0.013036026098982294</v>
+        <v>1.3036026098982294E-2</v>
       </c>
       <c r="G228">
-        <v>0.718723244358937</v>
+        <v>0.71872324435893697</v>
       </c>
       <c r="H228">
-        <v>0.2812767556410631</v>
+        <v>0.28127675564106308</v>
       </c>
       <c r="I228">
         <v>-0.11519261494163333</v>
@@ -1746,7 +1748,7 @@
         <v>1.1151926149416334</v>
       </c>
     </row>
-    <row r="230" spans="1:10">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>37</v>
       </c>
@@ -1754,31 +1756,31 @@
         <v>11</v>
       </c>
       <c r="C230">
-        <v>0.036713980070703776</v>
+        <v>3.6713980070703776E-2</v>
       </c>
       <c r="D230">
-        <v>0.020160176021350965</v>
+        <v>2.0160176021350965E-2</v>
       </c>
       <c r="E230">
-        <v>0.02053056065423855</v>
+        <v>2.0530560654238549E-2</v>
       </c>
       <c r="F230">
-        <v>0.031787831234923354</v>
+        <v>3.1787831234923354E-2</v>
       </c>
       <c r="G230">
-        <v>0.9776254067171911</v>
+        <v>0.97762540671719111</v>
       </c>
       <c r="H230">
-        <v>0.02237459328280889</v>
+        <v>2.2374593282808889E-2</v>
       </c>
       <c r="I230">
         <v>0.29758409735271785</v>
       </c>
       <c r="J230">
-        <v>0.7024159026472822</v>
-      </c>
-    </row>
-    <row r="236" spans="1:10">
+        <v>0.70241590264728215</v>
+      </c>
+    </row>
+    <row r="236" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>38</v>
       </c>
@@ -1786,19 +1788,19 @@
         <v>11</v>
       </c>
       <c r="C236">
-        <v>0.015642009092624462</v>
+        <v>1.5642009092624462E-2</v>
       </c>
       <c r="D236">
-        <v>0.020474991686462492</v>
+        <v>2.0474991686462492E-2</v>
       </c>
       <c r="E236">
-        <v>0.019116533096558946</v>
+        <v>1.9116533096558946E-2</v>
       </c>
       <c r="F236">
-        <v>0.016201568733618592</v>
+        <v>1.6201568733618592E-2</v>
       </c>
       <c r="G236">
-        <v>0.7189192049572954</v>
+        <v>0.71891920495729544</v>
       </c>
       <c r="H236">
         <v>0.28108079504270456</v>
@@ -1807,10 +1809,10 @@
         <v>0.11577936194257338</v>
       </c>
       <c r="J236">
-        <v>0.8842206380574266</v>
-      </c>
-    </row>
-    <row r="238" spans="1:10">
+        <v>0.88422063805742657</v>
+      </c>
+    </row>
+    <row r="238" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>39</v>
       </c>
@@ -1818,19 +1820,19 @@
         <v>11</v>
       </c>
       <c r="C238">
-        <v>0.022325140684470245</v>
+        <v>2.2325140684470245E-2</v>
       </c>
       <c r="D238">
-        <v>0.011736942477963587</v>
+        <v>1.1736942477963587E-2</v>
       </c>
       <c r="E238">
-        <v>0.012901160956049115</v>
+        <v>1.2901160956049115E-2</v>
       </c>
       <c r="F238">
-        <v>0.0209501248731893</v>
+        <v>2.0950124873189299E-2</v>
       </c>
       <c r="G238">
-        <v>0.8900456474860763</v>
+        <v>0.89004564748607629</v>
       </c>
       <c r="H238">
         <v>0.10995435251392369</v>
@@ -1839,10 +1841,10 @@
         <v>0.12986305927253713</v>
       </c>
       <c r="J238">
-        <v>0.8701369407274628</v>
-      </c>
-    </row>
-    <row r="242" spans="1:10">
+        <v>0.87013694072746284</v>
+      </c>
+    </row>
+    <row r="242" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>40</v>
       </c>
@@ -1850,31 +1852,31 @@
         <v>11</v>
       </c>
       <c r="C242">
-        <v>0.022233368993100106</v>
+        <v>2.2233368993100106E-2</v>
       </c>
       <c r="D242">
-        <v>0.025763446141393764</v>
+        <v>2.5763446141393764E-2</v>
       </c>
       <c r="E242">
-        <v>0.02604247122673491</v>
+        <v>2.604247122673491E-2</v>
       </c>
       <c r="F242">
-        <v>0.02199342941485015</v>
+        <v>2.1993429414850149E-2</v>
       </c>
       <c r="G242">
         <v>1.0790422060537739</v>
       </c>
       <c r="H242">
-        <v>-0.07904220605377395</v>
+        <v>-7.9042206053773947E-2</v>
       </c>
       <c r="I242">
-        <v>-0.06797006642360112</v>
+        <v>-6.7970066423601122E-2</v>
       </c>
       <c r="J242">
         <v>1.0679700664236011</v>
       </c>
     </row>
-    <row r="246" spans="1:10">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>41</v>
       </c>
@@ -1882,19 +1884,19 @@
         <v>11</v>
       </c>
       <c r="C246">
-        <v>0.0065884828950483485</v>
+        <v>6.5884828950483485E-3</v>
       </c>
       <c r="D246">
-        <v>0.015311446411769455</v>
+        <v>1.5311446411769455E-2</v>
       </c>
       <c r="E246">
-        <v>0.011370551730549065</v>
+        <v>1.1370551730549065E-2</v>
       </c>
       <c r="F246">
-        <v>0.00790489244546335</v>
+        <v>7.9048924454633504E-3</v>
       </c>
       <c r="G246">
-        <v>0.5482160766044633</v>
+        <v>0.54821607660446325</v>
       </c>
       <c r="H246">
         <v>0.45178392339553664</v>
@@ -1903,10 +1905,10 @@
         <v>0.15091310973519123</v>
       </c>
       <c r="J246">
-        <v>0.8490868902648087</v>
-      </c>
-    </row>
-    <row r="248" spans="1:10">
+        <v>0.84908689026480866</v>
+      </c>
+    </row>
+    <row r="248" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>42</v>
       </c>
@@ -1914,31 +1916,31 @@
         <v>11</v>
       </c>
       <c r="C248">
-        <v>0.028687253999607993</v>
+        <v>2.8687253999607993E-2</v>
       </c>
       <c r="D248">
-        <v>0.01941238474001075</v>
+        <v>1.9412384740010748E-2</v>
       </c>
       <c r="E248">
-        <v>0.02219076536688332</v>
+        <v>2.219076536688332E-2</v>
       </c>
       <c r="F248">
-        <v>0.026257136884691654</v>
+        <v>2.6257136884691654E-2</v>
       </c>
       <c r="G248">
-        <v>0.7004399146653609</v>
+        <v>0.70043991466536093</v>
       </c>
       <c r="H248">
-        <v>0.2995600853346391</v>
+        <v>0.29956008533463913</v>
       </c>
       <c r="I248">
         <v>0.26201092941571724</v>
       </c>
       <c r="J248">
-        <v>0.7379890705842828</v>
-      </c>
-    </row>
-    <row r="250" spans="1:10">
+        <v>0.73798907058428276</v>
+      </c>
+    </row>
+    <row r="250" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>43</v>
       </c>
@@ -1946,31 +1948,31 @@
         <v>11</v>
       </c>
       <c r="C250">
-        <v>0.01823046536636357</v>
+        <v>1.8230465366363569E-2</v>
       </c>
       <c r="D250">
-        <v>0.016271969155495076</v>
+        <v>1.6271969155495076E-2</v>
       </c>
       <c r="E250">
-        <v>0.017868406436898958</v>
+        <v>1.7868406436898958E-2</v>
       </c>
       <c r="F250">
-        <v>0.01842396993899686</v>
+        <v>1.8423969938996861E-2</v>
       </c>
       <c r="G250">
         <v>0.18486577990572503</v>
       </c>
       <c r="H250">
-        <v>0.8151342200942749</v>
+        <v>0.81513422009427494</v>
       </c>
       <c r="I250">
-        <v>-0.09880262803647838</v>
+        <v>-9.8802628036478379E-2</v>
       </c>
       <c r="J250">
         <v>1.0988026280364784</v>
       </c>
     </row>
-    <row r="256" spans="1:10">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>44</v>
       </c>
@@ -1978,19 +1980,19 @@
         <v>11</v>
       </c>
       <c r="C256">
-        <v>0.027132078393627287</v>
+        <v>2.7132078393627287E-2</v>
       </c>
       <c r="D256">
-        <v>0.021548543926225988</v>
+        <v>2.1548543926225988E-2</v>
       </c>
       <c r="E256">
-        <v>0.029295231680833565</v>
+        <v>2.9295231680833565E-2</v>
       </c>
       <c r="F256">
-        <v>0.021137073546287077</v>
+        <v>2.1137073546287077E-2</v>
       </c>
       <c r="G256">
-        <v>-0.3874164832035248</v>
+        <v>-0.38741648320352479</v>
       </c>
       <c r="H256">
         <v>1.3874164832035247</v>
@@ -1999,10 +2001,10 @@
         <v>1.0736935327150257</v>
       </c>
       <c r="J256">
-        <v>-0.07369353271502561</v>
-      </c>
-    </row>
-    <row r="258" spans="1:10">
+        <v>-7.3693532715025614E-2</v>
+      </c>
+    </row>
+    <row r="258" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>45</v>
       </c>
@@ -2010,31 +2012,31 @@
         <v>11</v>
       </c>
       <c r="C258">
-        <v>0.03010459824599547</v>
+        <v>3.010459824599547E-2</v>
       </c>
       <c r="D258">
-        <v>0.019679927226808343</v>
+        <v>1.9679927226808343E-2</v>
       </c>
       <c r="E258">
-        <v>0.023580476765924268</v>
+        <v>2.3580476765924268E-2</v>
       </c>
       <c r="F258">
-        <v>0.024698136783082893</v>
+        <v>2.4698136783082893E-2</v>
       </c>
       <c r="G258">
-        <v>0.6258347594915208</v>
+        <v>0.62583475949152079</v>
       </c>
       <c r="H258">
         <v>0.37416524050847927</v>
       </c>
       <c r="I258">
-        <v>0.5186217822089269</v>
+        <v>0.51862178220892685</v>
       </c>
       <c r="J258">
         <v>0.4813782177910732</v>
       </c>
     </row>
-    <row r="260" spans="1:10">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>47</v>
       </c>
@@ -2042,19 +2044,19 @@
         <v>11</v>
       </c>
       <c r="C260">
-        <v>0.028076625443192282</v>
+        <v>2.8076625443192282E-2</v>
       </c>
       <c r="D260">
-        <v>0.021277716809636013</v>
+        <v>2.1277716809636013E-2</v>
       </c>
       <c r="E260">
-        <v>0.022286505671257707</v>
+        <v>2.2286505671257707E-2</v>
       </c>
       <c r="F260">
-        <v>0.027140831508800662</v>
+        <v>2.7140831508800662E-2</v>
       </c>
       <c r="G260">
-        <v>0.8516248833463096</v>
+        <v>0.85162488334630959</v>
       </c>
       <c r="H260">
         <v>0.14837511665369038</v>
@@ -2063,10 +2065,10 @@
         <v>0.13763884541306737</v>
       </c>
       <c r="J260">
-        <v>0.8623611545869326</v>
-      </c>
-    </row>
-    <row r="262" spans="1:10">
+        <v>0.86236115458693263</v>
+      </c>
+    </row>
+    <row r="262" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>48</v>
       </c>
@@ -2074,19 +2076,19 @@
         <v>11</v>
       </c>
       <c r="C262">
-        <v>0.018703336218479416</v>
+        <v>1.8703336218479416E-2</v>
       </c>
       <c r="D262">
-        <v>0.02842446157065702</v>
+        <v>2.842446157065702E-2</v>
       </c>
       <c r="E262">
-        <v>0.02497008413473442</v>
+        <v>2.4970084134734422E-2</v>
       </c>
       <c r="F262">
-        <v>0.021473161890909392</v>
+        <v>2.1473161890909392E-2</v>
       </c>
       <c r="G262">
-        <v>0.6446525159611493</v>
+        <v>0.64465251596114925</v>
       </c>
       <c r="H262">
         <v>0.35534748403885075</v>
@@ -2095,10 +2097,10 @@
         <v>0.28492850077378284</v>
       </c>
       <c r="J262">
-        <v>0.7150714992262172</v>
-      </c>
-    </row>
-    <row r="268" spans="1:10">
+        <v>0.71507149922621716</v>
+      </c>
+    </row>
+    <row r="268" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>49</v>
       </c>
@@ -2106,31 +2108,31 @@
         <v>11</v>
       </c>
       <c r="C268">
-        <v>0.018398560525665787</v>
+        <v>1.8398560525665787E-2</v>
       </c>
       <c r="D268">
-        <v>0.021700490001798408</v>
+        <v>2.1700490001798408E-2</v>
       </c>
       <c r="E268">
-        <v>0.02211403427578253</v>
+        <v>2.211403427578253E-2</v>
       </c>
       <c r="F268">
-        <v>0.018203498165186186</v>
+        <v>1.8203498165186186E-2</v>
       </c>
       <c r="G268">
         <v>1.125243218237503</v>
       </c>
       <c r="H268">
-        <v>-0.125243218237503</v>
+        <v>-0.12524321823750301</v>
       </c>
       <c r="I268">
-        <v>-0.05907526550447915</v>
+        <v>-5.9075265504479148E-2</v>
       </c>
       <c r="J268">
-        <v>1.059075265504479</v>
-      </c>
-    </row>
-    <row r="270" spans="1:10">
+        <v>1.0590752655044791</v>
+      </c>
+    </row>
+    <row r="270" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>50</v>
       </c>
@@ -2138,28 +2140,28 @@
         <v>11</v>
       </c>
       <c r="C270">
-        <v>0.024499678906257996</v>
+        <v>2.4499678906257996E-2</v>
       </c>
       <c r="D270">
-        <v>0.012953465027957484</v>
+        <v>1.2953465027957484E-2</v>
       </c>
       <c r="E270">
-        <v>0.014829119660668503</v>
+        <v>1.4829119660668503E-2</v>
       </c>
       <c r="F270">
-        <v>0.021461838965840162</v>
+        <v>2.1461838965840162E-2</v>
       </c>
       <c r="G270">
-        <v>0.8375524087392796</v>
+        <v>0.83755240873927961</v>
       </c>
       <c r="H270">
         <v>0.16244759126072034</v>
       </c>
       <c r="I270">
-        <v>0.2631026908419762</v>
+        <v>0.26310269084197618</v>
       </c>
       <c r="J270">
-        <v>0.7368973091580238</v>
+        <v>0.73689730915802376</v>
       </c>
     </row>
   </sheetData>

</xml_diff>